<commit_message>
testing report card visualization  methods
</commit_message>
<xml_diff>
--- a/data/test_table.xlsx
+++ b/data/test_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{942D963A-5242-40E3-8F86-0FF9B67F2E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096999EB-0057-4BA4-958F-C26CC20F3E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
+    <workbookView xWindow="2430" yWindow="3750" windowWidth="21600" windowHeight="11295" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Indicator (units)</t>
   </si>
@@ -48,23 +48,101 @@
     <t>Time Series</t>
   </si>
   <si>
-    <t>Mean winter (Feb-Mar) bottom temperature - North (°C)</t>
-  </si>
-  <si>
-    <t>Below threshold</t>
-  </si>
-  <si>
-    <t>Cold winter temperatures may increase the mortality of young-of-the-year fish, resulting in smaller year classes. 2024 temperature was colder than black sea bass's lower threshold of 8C. Bottom temperature data comes from GLORYS, a modeled product.</t>
-  </si>
-  <si>
-    <t>winter bottom temp North_2025-02-10.png</t>
+    <t>Mean winter (Feb-Mar) bottom temperature (°C)</t>
+  </si>
+  <si>
+    <t>Cold winter temperatures may increase the mortality of young-of-the-year fish, resulting in smaller year classes. Additionally, cold temperatures can cause northern fish to move into the southern subregion, leading to potential misallocation of catch between the northern and southern stock subunits. 2024 temperature in the northern subunit (north of Hudson Canyon) was colder than black sea bass's lower threshold of 8C. Bottom temperature data comes from GLORYS, a modeled product.</t>
+  </si>
+  <si>
+    <t>N/A (no data for 2024)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Shelf water volume is a proxy for suitable winter habitat; higher shelf water volume indicates less suitable habitat, potentially leading to northern fish migrating into the southern subregion. The shelf water volume dataset is created from </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>in situ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> data, and there has been no winter sampling since 2021, highlighting the need for additional indicators to inform stock subunit mixing.</t>
+    </r>
+  </si>
+  <si>
+    <t>MRIP recreational trips (millions of annual trips)</t>
+  </si>
+  <si>
+    <t>Recent trip numbers are near an all-time high, but may have decreased from 2023 (2024 data is preliminary and does not include November and December 2024). Catch (not shown) generally reflects trip patterns. High regulatory complexity is likely contributing to recreational fishing trends.</t>
+  </si>
+  <si>
+    <t>MRIP recreational landings (millions of lbs.)</t>
+  </si>
+  <si>
+    <t>The recreational black sea bass fishery has a catch-and-release component, and management measures are being implemented to reduce recreational harvest. 2024 data is preliminary and does not include November and December 2024.</t>
+  </si>
+  <si>
+    <t>Commercial revenue per vessel (2023 USD)</t>
+  </si>
+  <si>
+    <t>Commercial revenue per vessel has an overall increasing trend, suggesting potentially favorable returns in the fishery, despite decreases in both total landings and average price ($/lb.; not shown).</t>
+  </si>
+  <si>
+    <t>Number of commercial vessels (#)</t>
+  </si>
+  <si>
+    <t>The number of active vessels has been decreasing since 2017, which could impact revenue distributions and fleet composition. </t>
+  </si>
+  <si>
+    <t>Shelf water volume (km3)</t>
+  </si>
+  <si>
+    <t>bt_facet.png</t>
+  </si>
+  <si>
+    <t>swv_facet.png</t>
+  </si>
+  <si>
+    <t>total_recreational_trips_n_millions_2025-02-18.png</t>
+  </si>
+  <si>
+    <t>total_recreational_landings_lbs_millions_2025-02-18.png</t>
+  </si>
+  <si>
+    <t>AVGVESREVperYr_BLACK_SEABASS_2023_DOLlb_2025-02-18.png</t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_BLACK_SEABASS_2025-02-18.png</t>
+  </si>
+  <si>
+    <t>North: Below threshold South: Near long-term average</t>
+  </si>
+  <si>
+    <t>Above long-term average</t>
+  </si>
+  <si>
+    <t>Near long-term average</t>
+  </si>
+  <si>
+    <t>Below long-term average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +163,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,15 +218,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,40 +544,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616C184B-97FE-4AFC-A455-4B1A01E2E914}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test report card table rendering
</commit_message>
<xml_diff>
--- a/data/test_table.xlsx
+++ b/data/test_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096999EB-0057-4BA4-958F-C26CC20F3E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDC40C3-45BD-4B8B-92F1-DB6B94145A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="3750" windowWidth="21600" windowHeight="11295" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
+    <workbookView xWindow="-25695" yWindow="-675" windowWidth="21600" windowHeight="11295" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Indicator (units)</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Below long-term average</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -226,10 +232,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,32 +550,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616C184B-97FE-4AFC-A455-4B1A01E2E914}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -582,8 +594,14 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -596,8 +614,14 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -610,8 +634,14 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -624,8 +654,14 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -638,8 +674,14 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -651,6 +693,12 @@
       </c>
       <c r="D7" t="s">
         <v>22</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update report card template
</commit_message>
<xml_diff>
--- a/data/test_table.xlsx
+++ b/data/test_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDC40C3-45BD-4B8B-92F1-DB6B94145A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8EE156-48E3-4F00-A046-B7BE4F690644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25695" yWindow="-675" windowWidth="21600" windowHeight="11295" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
+    <workbookView xWindow="1455" yWindow="2055" windowWidth="21600" windowHeight="11235" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>